<commit_message>
New samples for new sample data list.
</commit_message>
<xml_diff>
--- a/samples/sample.xlsx
+++ b/samples/sample.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
   <si>
     <t>[Input]</t>
   </si>
@@ -128,10 +128,28 @@
     <t>tumor</t>
   </si>
   <si>
+    <t>control</t>
+  </si>
+  <si>
     <t>s_B2Na;s_B2Nb</t>
   </si>
   <si>
+    <t>List1</t>
+  </si>
+  <si>
     <t>s_B3Ta;s_B3Tb</t>
+  </si>
+  <si>
+    <t>List2</t>
+  </si>
+  <si>
+    <t>[ControlPanel]</t>
+  </si>
+  <si>
+    <t>s_B1N,s_B2Na, s_B2Nb, s_B3N, s_B4N</t>
+  </si>
+  <si>
+    <t>s_B3N, s_B4N</t>
   </si>
   <si>
     <t>#s_B1N  s_B1T  s_B2Na  s_B2Nb  s_B2T  s_B3N  s_B3Ta  s_B3Tb  s_B4N  s_B4Ta  s_B4Tb  s_B5N  s_B6T  s_B7T</t>
@@ -209,9 +227,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -231,10 +253,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -383,6 +405,9 @@
       <c r="B16" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="C16" s="0" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -394,10 +419,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>16</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -405,7 +433,10 @@
         <v>19</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -415,10 +446,44 @@
       <c r="B20" s="0" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="C20" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
         <v>39</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>